<commit_message>
Spreadsheets in .xlsx format of paths to audiofiles
</commit_message>
<xml_diff>
--- a/csv-spreadsheets/noises.xlsx
+++ b/csv-spreadsheets/noises.xlsx
@@ -19,399 +19,753 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="249">
   <si>
     <t>filename</t>
   </si>
   <si>
-    <t>./ms-snsd/noise_train/AirConditioner_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirConditioner_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_11.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/AirportAnnouncement_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_11.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Babble_12.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Bus_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Cafe_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CafeTeria_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Car_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/CopyMachine_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Field_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Hallway_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Kitchen_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/LivingRoom_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Metro_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Munching_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_11.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_12.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_13.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/NeighborSpeaking_14.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Office_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Park_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Restaurant_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/ShuttingDoor_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Square_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/SqueakyChair_11.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Station_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Traffic_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Typing_10.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_8.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/VacuumCleaner_9.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/WasherDryer_1.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/WasherDryer_2.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/WasherDryer_3.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/WasherDryer_4.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/WasherDryer_5.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/WasherDryer_6.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/WasherDryer_7.wav</t>
-  </si>
-  <si>
-    <t>./ms-snsd/noise_train/Washing_7.wav</t>
+    <t>./ms-snsd/Noise_training/noisy1_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy1_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy1_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy1_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy2_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy2_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy2_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy2_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy3_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy3_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy3_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy3_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy4_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy4_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy4_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy4_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy5_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy5_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy5_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy5_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy6_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy6_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy6_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy6_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy7_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy7_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy7_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy7_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy8_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy8_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy8_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy8_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy9_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy9_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy9_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy9_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy10_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy10_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy10_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy10_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy11_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy11_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy11_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy11_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy12_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy12_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy12_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy12_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy13_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy13_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy13_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy13_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy14_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy14_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy14_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy14_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy15_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy15_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy15_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy15_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy16_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy16_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy16_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy16_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy17_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy17_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy17_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy17_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy18_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy18_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy18_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy18_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy19_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy19_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy19_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy19_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy20_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy20_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy20_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy20_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy21_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy21_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy21_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy21_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy22_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy22_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy22_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy22_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy23_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy23_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy23_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy23_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy24_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy24_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy24_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy24_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy25_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy25_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy25_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy25_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy26_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy26_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy26_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy26_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy27_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy27_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy27_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy27_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy28_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy28_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy28_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy28_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy29_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy29_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy29_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy29_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy30_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy30_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy30_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy30_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy31_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy31_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy31_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy31_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy32_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy32_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy32_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy32_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy33_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy33_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy33_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy33_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy34_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy34_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy34_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy34_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy35_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy35_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy35_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy35_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy36_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy36_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy36_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy36_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy37_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy37_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy37_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy37_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy38_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy38_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy38_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy38_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy39_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy39_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy39_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy39_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy40_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy40_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy40_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy40_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy41_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy41_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy41_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy41_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy42_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy42_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy42_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy42_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy43_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy43_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy43_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy43_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy44_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy44_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy44_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy44_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy45_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy45_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy45_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy45_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy46_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy46_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy46_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy46_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy47_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy47_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy47_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy47_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy48_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy48_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy48_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy48_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy49_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy49_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy49_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy49_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy50_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy50_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy50_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy50_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy51_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy51_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy51_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy51_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy52_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy52_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy52_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy52_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy53_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy53_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy53_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy53_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy54_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy54_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy54_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy54_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy55_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy55_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy55_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy55_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy56_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy56_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy56_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy56_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy57_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy57_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy57_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy57_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy58_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy58_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy58_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy58_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy59_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy59_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy59_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy59_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy60_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy60_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy60_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy60_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy61_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy61_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy61_SNRdb_30.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy61_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy62_SNRdb_0.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy62_SNRdb_10.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy62_SNRdb_20.0.wav</t>
+  </si>
+  <si>
+    <t>./ms-snsd/Noise_training/noisy62_SNRdb_30.0.wav</t>
   </si>
 </sst>
 </file>
@@ -729,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A131"/>
+  <dimension ref="A1:A249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="A249" sqref="A249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1395,6 +1749,596 @@
         <v>130</v>
       </c>
     </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>